<commit_message>
Revised participant account generation
</commit_message>
<xml_diff>
--- a/main/participant_kernel_accounts.xlsx
+++ b/main/participant_kernel_accounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18602d6f4978f644/Ayaz Lab/KernelFlow_PsychoPy/main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_669DB4BB87D0D653B77B2111595ED87656CDA317" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F62A3F1-C3F4-4F36-8981-D40756C7ECCA}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_1DEDB5A487005F7DFB582E11595ED87656CD7391" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A3E9287-7DC7-4F0C-9046-43073E2BA984}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,451 +34,451 @@
     <t>participant_01</t>
   </si>
   <si>
-    <t>participant_01_415873@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_01_415873!</t>
+    <t>participant.01.871072@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.01.871072!</t>
   </si>
   <si>
     <t>participant_02</t>
   </si>
   <si>
-    <t>participant_02_497719@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_02_497719!</t>
+    <t>participant.02.168920@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.02.168920!</t>
   </si>
   <si>
     <t>participant_03</t>
   </si>
   <si>
-    <t>participant_03_303054@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_03_303054!</t>
+    <t>participant.03.196494@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.03.196494!</t>
   </si>
   <si>
     <t>participant_04</t>
   </si>
   <si>
-    <t>participant_04_872243@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_04_872243!</t>
+    <t>participant.04.775601@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.04.775601!</t>
   </si>
   <si>
     <t>participant_05</t>
   </si>
   <si>
-    <t>participant_05_128890@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_05_128890!</t>
+    <t>participant.05.148398@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.05.148398!</t>
   </si>
   <si>
     <t>participant_06</t>
   </si>
   <si>
-    <t>participant_06_809482@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_06_809482!</t>
+    <t>participant.06.817205@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.06.817205!</t>
   </si>
   <si>
     <t>participant_07</t>
   </si>
   <si>
-    <t>participant_07_329546@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_07_329546!</t>
+    <t>participant.07.336639@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.07.336639!</t>
   </si>
   <si>
     <t>participant_08</t>
   </si>
   <si>
-    <t>participant_08_841528@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_08_841528!</t>
+    <t>participant.08.426113@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.08.426113!</t>
   </si>
   <si>
     <t>participant_09</t>
   </si>
   <si>
-    <t>participant_09_719838@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_09_719838!</t>
+    <t>participant.09.936550@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.09.936550!</t>
   </si>
   <si>
     <t>participant_10</t>
   </si>
   <si>
-    <t>participant_10_542507@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_10_542507!</t>
+    <t>participant.10.164237@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.10.164237!</t>
   </si>
   <si>
     <t>participant_11</t>
   </si>
   <si>
-    <t>participant_11_549125@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_11_549125!</t>
+    <t>participant.11.690825@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.11.690825!</t>
   </si>
   <si>
     <t>participant_12</t>
   </si>
   <si>
-    <t>participant_12_559455@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_12_559455!</t>
+    <t>participant.12.477502@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.12.477502!</t>
   </si>
   <si>
     <t>participant_13</t>
   </si>
   <si>
-    <t>participant_13_719058@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_13_719058!</t>
+    <t>participant.13.838504@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.13.838504!</t>
   </si>
   <si>
     <t>participant_14</t>
   </si>
   <si>
-    <t>participant_14_923390@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_14_923390!</t>
+    <t>participant.14.867888@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.14.867888!</t>
   </si>
   <si>
     <t>participant_15</t>
   </si>
   <si>
-    <t>participant_15_414415@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_15_414415!</t>
+    <t>participant.15.807057@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.15.807057!</t>
   </si>
   <si>
     <t>participant_16</t>
   </si>
   <si>
-    <t>participant_16_537557@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_16_537557!</t>
+    <t>participant.16.920743@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.16.920743!</t>
   </si>
   <si>
     <t>participant_17</t>
   </si>
   <si>
-    <t>participant_17_275763@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_17_275763!</t>
+    <t>participant.17.148791@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.17.148791!</t>
   </si>
   <si>
     <t>participant_18</t>
   </si>
   <si>
-    <t>participant_18_609316@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_18_609316!</t>
+    <t>participant.18.999408@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.18.999408!</t>
   </si>
   <si>
     <t>participant_19</t>
   </si>
   <si>
-    <t>participant_19_989686@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_19_989686!</t>
+    <t>participant.19.359380@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.19.359380!</t>
   </si>
   <si>
     <t>participant_20</t>
   </si>
   <si>
-    <t>participant_20_626125@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_20_626125!</t>
+    <t>participant.20.518840@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.20.518840!</t>
   </si>
   <si>
     <t>participant_21</t>
   </si>
   <si>
-    <t>participant_21_781283@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_21_781283!</t>
+    <t>participant.21.712896@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.21.712896!</t>
   </si>
   <si>
     <t>participant_22</t>
   </si>
   <si>
-    <t>participant_22_350924@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_22_350924!</t>
+    <t>participant.22.374905@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.22.374905!</t>
   </si>
   <si>
     <t>participant_23</t>
   </si>
   <si>
-    <t>participant_23_199184@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_23_199184!</t>
+    <t>participant.23.392599@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.23.392599!</t>
   </si>
   <si>
     <t>participant_24</t>
   </si>
   <si>
-    <t>participant_24_398675@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_24_398675!</t>
+    <t>participant.24.517838@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.24.517838!</t>
   </si>
   <si>
     <t>participant_25</t>
   </si>
   <si>
-    <t>participant_25_446928@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_25_446928!</t>
+    <t>participant.25.148636@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.25.148636!</t>
   </si>
   <si>
     <t>participant_26</t>
   </si>
   <si>
-    <t>participant_26_919567@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_26_919567!</t>
+    <t>participant.26.422165@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.26.422165!</t>
   </si>
   <si>
     <t>participant_27</t>
   </si>
   <si>
-    <t>participant_27_573024@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_27_573024!</t>
+    <t>participant.27.914784@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.27.914784!</t>
   </si>
   <si>
     <t>participant_28</t>
   </si>
   <si>
-    <t>participant_28_816368@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_28_816368!</t>
+    <t>participant.28.428654@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.28.428654!</t>
   </si>
   <si>
     <t>participant_29</t>
   </si>
   <si>
-    <t>participant_29_399441@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_29_399441!</t>
+    <t>participant.29.308663@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.29.308663!</t>
   </si>
   <si>
     <t>participant_30</t>
   </si>
   <si>
-    <t>participant_30_125919@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_30_125919!</t>
+    <t>participant.30.571415@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.30.571415!</t>
   </si>
   <si>
     <t>participant_31</t>
   </si>
   <si>
-    <t>participant_31_728027@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_31_728027!</t>
+    <t>participant.31.325825@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.31.325825!</t>
   </si>
   <si>
     <t>participant_32</t>
   </si>
   <si>
-    <t>participant_32_702834@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_32_702834!</t>
+    <t>participant.32.543356@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.32.543356!</t>
   </si>
   <si>
     <t>participant_33</t>
   </si>
   <si>
-    <t>participant_33_356560@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_33_356560!</t>
+    <t>participant.33.242590@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.33.242590!</t>
   </si>
   <si>
     <t>participant_34</t>
   </si>
   <si>
-    <t>participant_34_345568@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_34_345568!</t>
+    <t>participant.34.706355@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.34.706355!</t>
   </si>
   <si>
     <t>participant_35</t>
   </si>
   <si>
-    <t>participant_35_654161@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_35_654161!</t>
+    <t>participant.35.629305@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.35.629305!</t>
   </si>
   <si>
     <t>participant_36</t>
   </si>
   <si>
-    <t>participant_36_424489@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_36_424489!</t>
+    <t>participant.36.886970@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.36.886970!</t>
   </si>
   <si>
     <t>participant_37</t>
   </si>
   <si>
-    <t>participant_37_926525@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_37_926525!</t>
+    <t>participant.37.846949@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.37.846949!</t>
   </si>
   <si>
     <t>participant_38</t>
   </si>
   <si>
-    <t>participant_38_659067@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_38_659067!</t>
+    <t>participant.38.353984@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.38.353984!</t>
   </si>
   <si>
     <t>participant_39</t>
   </si>
   <si>
-    <t>participant_39_827869@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_39_827869!</t>
+    <t>participant.39.692211@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.39.692211!</t>
   </si>
   <si>
     <t>participant_40</t>
   </si>
   <si>
-    <t>participant_40_789966@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_40_789966!</t>
+    <t>participant.40.772216@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.40.772216!</t>
   </si>
   <si>
     <t>participant_41</t>
   </si>
   <si>
-    <t>participant_41_379405@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_41_379405!</t>
+    <t>participant.41.869391@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.41.869391!</t>
   </si>
   <si>
     <t>participant_42</t>
   </si>
   <si>
-    <t>participant_42_984491@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_42_984491!</t>
+    <t>participant.42.851273@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.42.851273!</t>
   </si>
   <si>
     <t>participant_43</t>
   </si>
   <si>
-    <t>participant_43_998950@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_43_998950!</t>
+    <t>participant.43.724103@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.43.724103!</t>
   </si>
   <si>
     <t>participant_44</t>
   </si>
   <si>
-    <t>participant_44_293501@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_44_293501!</t>
+    <t>participant.44.455580@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.44.455580!</t>
   </si>
   <si>
     <t>participant_45</t>
   </si>
   <si>
-    <t>participant_45_689689@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_45_689689!</t>
+    <t>participant.45.936288@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.45.936288!</t>
   </si>
   <si>
     <t>participant_46</t>
   </si>
   <si>
-    <t>participant_46_467856@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_46_467856!</t>
+    <t>participant.46.337060@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.46.337060!</t>
   </si>
   <si>
     <t>participant_47</t>
   </si>
   <si>
-    <t>participant_47_235917@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_47_235917!</t>
+    <t>participant.47.404964@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.47.404964!</t>
   </si>
   <si>
     <t>participant_48</t>
   </si>
   <si>
-    <t>participant_48_579809@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_48_579809!</t>
+    <t>participant.48.979720@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.48.979720!</t>
   </si>
   <si>
     <t>participant_49</t>
   </si>
   <si>
-    <t>participant_49_261691@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_49_261691!</t>
+    <t>participant.49.170686@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.49.170686!</t>
   </si>
   <si>
     <t>participant_50</t>
   </si>
   <si>
-    <t>participant_50_154845@gmail.com</t>
-  </si>
-  <si>
-    <t>Participant_50_154845!</t>
+    <t>participant.50.827863@gmail.com</t>
+  </si>
+  <si>
+    <t>Participant.50.827863!</t>
   </si>
 </sst>
 </file>
@@ -843,12 +843,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>